<commit_message>
Add data processing script for IE and UVA 2025 surveys and update Excel files
</commit_message>
<xml_diff>
--- a/Encuestas/IE.2025.xlsx
+++ b/Encuestas/IE.2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70254057\Downloads\final forms sg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\70254057\Desktop\basic-hub\LocalWealthHousing\Encuestas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB67A1A2-DEB4-4FAC-8152-5091B2CC24E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4FADB80-01E2-45F0-9B99-3657E5D2D651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -586,9 +586,6 @@
     <t>hora_de_inicio</t>
   </si>
   <si>
-    <t>hora_de_finalización</t>
-  </si>
-  <si>
     <t>correo_electrónico</t>
   </si>
   <si>
@@ -647,6 +644,9 @@
   </si>
   <si>
     <t>48 months</t>
+  </si>
+  <si>
+    <t>hora_de_finalizacion</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,10 +1064,10 @@
         <v>187</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1079,49 +1079,49 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -1150,7 +1150,7 @@
         <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>53</v>
@@ -1212,7 +1212,7 @@
         <v>46</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>54</v>
@@ -1345,7 +1345,7 @@
         <v>46</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>53</v>
@@ -1413,7 +1413,7 @@
         <v>46</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>55</v>
@@ -1478,7 +1478,7 @@
         <v>46</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>55</v>
@@ -1543,7 +1543,7 @@
         <v>46</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>55</v>
@@ -1608,7 +1608,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>53</v>
@@ -1676,7 +1676,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>55</v>
@@ -1738,7 +1738,7 @@
         <v>47</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>55</v>
@@ -1806,7 +1806,7 @@
         <v>46</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>53</v>
@@ -2004,7 +2004,7 @@
         <v>46</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>55</v>
@@ -2069,7 +2069,7 @@
         <v>46</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>55</v>
@@ -2131,7 +2131,7 @@
         <v>46</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>53</v>
@@ -2190,7 +2190,7 @@
         <v>46</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>53</v>
@@ -2252,7 +2252,7 @@
         <v>46</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J19" s="2" t="s">
         <v>55</v>
@@ -2441,7 +2441,7 @@
         <v>46</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>56</v>
@@ -2485,7 +2485,7 @@
         <v>46</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>54</v>
@@ -2547,7 +2547,7 @@
         <v>46</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>55</v>
@@ -2609,7 +2609,7 @@
         <v>46</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>53</v>
@@ -2665,7 +2665,7 @@
         <v>46</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>55</v>
@@ -2730,7 +2730,7 @@
         <v>46</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J27" s="2" t="s">
         <v>55</v>
@@ -2795,7 +2795,7 @@
         <v>46</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>54</v>
@@ -2863,7 +2863,7 @@
         <v>46</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>53</v>
@@ -2925,7 +2925,7 @@
         <v>46</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>54</v>
@@ -2987,7 +2987,7 @@
         <v>46</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>55</v>
@@ -3049,7 +3049,7 @@
         <v>46</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>55</v>
@@ -3114,7 +3114,7 @@
         <v>46</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>53</v>
@@ -3785,7 +3785,7 @@
         <v>46</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>53</v>
@@ -3921,7 +3921,7 @@
         <v>46</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J45" s="2" t="s">
         <v>55</v>
@@ -3989,7 +3989,7 @@
         <v>46</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>53</v>
@@ -4125,7 +4125,7 @@
         <v>46</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>53</v>
@@ -4261,7 +4261,7 @@
         <v>46</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>55</v>

</xml_diff>